<commit_message>
Updated WBP_Canteen | Imported 2 Images (Marco)
Two versions with switching backgrounds and transparency added in pep for kids
</commit_message>
<xml_diff>
--- a/Food Requirements.xlsx
+++ b/Food Requirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/29700CA7A5A595D9/Dokumenty/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\ProjectIndiana\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{7040B4E9-BEEC-4BFA-B411-FBF14BCB2367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DDAE045-E8FB-4786-B0A4-1A379AFD79F0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D44C3BE-ACEE-4D4F-BAF7-11E305FB3C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20520" yWindow="5265" windowWidth="20640" windowHeight="11040" xr2:uid="{04F22E59-84AB-4130-92E6-A304CF777A2C}"/>
+    <workbookView xWindow="-20520" yWindow="9180" windowWidth="16650" windowHeight="10905" xr2:uid="{04F22E59-84AB-4130-92E6-A304CF777A2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -135,7 +135,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,7 +168,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -503,15 +503,16 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="30.85546875" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -522,7 +523,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -533,7 +534,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -544,7 +545,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -555,7 +556,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -566,7 +567,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -577,7 +578,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -588,7 +589,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -599,7 +600,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -610,7 +611,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -621,7 +622,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -632,7 +633,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -643,7 +644,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -654,7 +655,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -665,7 +666,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -676,7 +677,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -687,7 +688,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -698,7 +699,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -709,7 +710,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>

</xml_diff>